<commit_message>
Docs:  update md files
Update md files.
</commit_message>
<xml_diff>
--- a/uefa_euro_2016_goalkeeping_stats.xlsx
+++ b/uefa_euro_2016_goalkeeping_stats.xlsx
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1359,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>